<commit_message>
updated the invoice template with the signature
</commit_message>
<xml_diff>
--- a/Yazle_Invoice_Template_Final.xlsx
+++ b/Yazle_Invoice_Template_Final.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Yazle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://napptix-my.sharepoint.com/personal/abhishek_napptix_com/Documents/Codefiles/InoviceTemplatation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E404EA-60AE-4E13-A5B6-7416E1724A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{F3E404EA-60AE-4E13-A5B6-7416E1724A32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4FDC3906-6FDC-4328-9E2C-C458CBC38FC0}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Invoice" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="55">
   <si>
     <t>Yazle Marketing Management LLC</t>
   </si>
@@ -799,6 +799,50 @@
             </a14:hiddenFill>
           </a:ext>
         </a:extLst>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>246654</xdr:colOff>
+      <xdr:row>30</xdr:row>
+      <xdr:rowOff>36736</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>5</xdr:col>
+      <xdr:colOff>652565</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>44532</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1BBF4EBE-D904-A9B4-247C-1A6BABBC2236}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5379133" y="5578554"/>
+          <a:ext cx="1733639" cy="558829"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
       </xdr:spPr>
     </xdr:pic>
     <xdr:clientData/>
@@ -1094,24 +1138,24 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:G46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="121" zoomScaleNormal="113" zoomScaleSheetLayoutView="36" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29:C37"/>
+    <sheetView tabSelected="1" topLeftCell="A21" zoomScale="121" zoomScaleNormal="113" zoomScaleSheetLayoutView="36" workbookViewId="0">
+      <selection activeCell="H33" sqref="H33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="16.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="41.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.7109375" style="1" customWidth="1"/>
-    <col min="7" max="7" width="9.140625" style="1"/>
-    <col min="8" max="8" width="12.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="16.1796875" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="41.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.1796875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.7265625" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.1796875" style="1"/>
+    <col min="8" max="8" width="12.81640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" s="3"/>
       <c r="B1" s="73" t="s">
         <v>50</v>
@@ -1122,7 +1166,7 @@
       <c r="F1" s="75"/>
       <c r="G1" s="3"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A2" s="3"/>
       <c r="B2" s="4"/>
       <c r="C2" s="5"/>
@@ -1131,7 +1175,7 @@
       <c r="F2" s="6"/>
       <c r="G2" s="3"/>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A3" s="3"/>
       <c r="B3" s="8"/>
       <c r="C3" s="29" t="s">
@@ -1141,7 +1185,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="3"/>
     </row>
-    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3"/>
       <c r="B4" s="8"/>
       <c r="C4" s="32" t="s">
@@ -1151,7 +1195,7 @@
       <c r="F4" s="9"/>
       <c r="G4" s="3"/>
     </row>
-    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3"/>
       <c r="B5" s="8"/>
       <c r="C5" s="32" t="s">
@@ -1161,7 +1205,7 @@
       <c r="F5" s="9"/>
       <c r="G5" s="3"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A6" s="3"/>
       <c r="B6" s="8"/>
       <c r="C6" s="31" t="s">
@@ -1171,7 +1215,7 @@
       <c r="F6" s="9"/>
       <c r="G6" s="3"/>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A7" s="3"/>
       <c r="B7" s="10"/>
       <c r="C7" s="33" t="s">
@@ -1181,7 +1225,7 @@
       <c r="F7" s="11"/>
       <c r="G7" s="3"/>
     </row>
-    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3"/>
       <c r="B8" s="12"/>
       <c r="C8" s="61" t="s">
@@ -1192,7 +1236,7 @@
       <c r="F8" s="13"/>
       <c r="G8" s="3"/>
     </row>
-    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="3"/>
       <c r="B9" s="14"/>
       <c r="C9" s="62"/>
@@ -1201,7 +1245,7 @@
       <c r="F9" s="15"/>
       <c r="G9" s="3"/>
     </row>
-    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3"/>
       <c r="B10" s="16"/>
       <c r="C10" s="63"/>
@@ -1210,7 +1254,7 @@
       <c r="F10" s="17"/>
       <c r="G10" s="3"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="18" t="s">
         <v>16</v>
@@ -1225,7 +1269,7 @@
       </c>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A12" s="3"/>
       <c r="B12" s="22" t="s">
         <v>3</v>
@@ -1242,7 +1286,7 @@
       </c>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="22" t="s">
         <v>4</v>
@@ -1260,7 +1304,7 @@
       </c>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="22"/>
       <c r="C14" s="42" t="s">
@@ -1275,7 +1319,7 @@
       </c>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A15" s="3"/>
       <c r="B15" s="22"/>
       <c r="C15" s="42" t="s">
@@ -1290,13 +1334,13 @@
       </c>
       <c r="G15" s="3"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A16" s="3"/>
       <c r="B16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="C16" s="24">
-        <v>100041433200003</v>
+      <c r="C16" s="24" t="s">
+        <v>0</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="22" t="s">
@@ -1307,7 +1351,7 @@
       </c>
       <c r="G16" s="3"/>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A17" s="3"/>
       <c r="B17" s="10"/>
       <c r="C17" s="25"/>
@@ -1316,7 +1360,7 @@
       <c r="F17" s="25"/>
       <c r="G17" s="3"/>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A18" s="3"/>
       <c r="B18" s="8"/>
       <c r="C18" s="3"/>
@@ -1325,7 +1369,7 @@
       <c r="F18" s="9"/>
       <c r="G18" s="3"/>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A19" s="3"/>
       <c r="B19" s="8"/>
       <c r="C19" s="3"/>
@@ -1334,7 +1378,7 @@
       <c r="F19" s="9"/>
       <c r="G19" s="3"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A20" s="3"/>
       <c r="B20" s="43" t="s">
         <v>5</v>
@@ -1353,7 +1397,7 @@
       </c>
       <c r="G20" s="3"/>
     </row>
-    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="3"/>
       <c r="B21" s="44">
         <v>1</v>
@@ -1373,7 +1417,7 @@
       </c>
       <c r="G21" s="3"/>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A22" s="3"/>
       <c r="B22" s="44"/>
       <c r="C22" s="41"/>
@@ -1382,7 +1426,7 @@
       <c r="F22" s="55"/>
       <c r="G22" s="3"/>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A23" s="3"/>
       <c r="B23" s="21"/>
       <c r="C23" s="41"/>
@@ -1391,7 +1435,7 @@
       <c r="F23" s="55"/>
       <c r="G23" s="3"/>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A24" s="3"/>
       <c r="B24" s="21"/>
       <c r="C24" s="47"/>
@@ -1400,7 +1444,7 @@
       <c r="F24" s="45"/>
       <c r="G24" s="3"/>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A25" s="3"/>
       <c r="B25" s="40"/>
       <c r="C25" s="27"/>
@@ -1414,7 +1458,7 @@
       </c>
       <c r="G25" s="3"/>
     </row>
-    <row r="26" spans="1:7" ht="22.5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A26" s="3"/>
       <c r="B26" s="2" t="s">
         <v>19</v>
@@ -1432,7 +1476,7 @@
       </c>
       <c r="G26" s="3"/>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A27" s="3"/>
       <c r="B27" s="49"/>
       <c r="C27" s="26"/>
@@ -1446,7 +1490,7 @@
       </c>
       <c r="G27" s="3"/>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A28" s="3"/>
       <c r="B28" s="50" t="s">
         <v>24</v>
@@ -1459,7 +1503,7 @@
       <c r="F28" s="78"/>
       <c r="G28" s="3"/>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A29" s="3"/>
       <c r="B29" s="8" t="s">
         <v>25</v>
@@ -1472,7 +1516,7 @@
       <c r="F29" s="81"/>
       <c r="G29" s="3"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A30" s="3"/>
       <c r="B30" s="8" t="s">
         <v>27</v>
@@ -1485,7 +1529,7 @@
       <c r="F30" s="84"/>
       <c r="G30" s="3"/>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A31" s="3"/>
       <c r="B31" s="8" t="s">
         <v>34</v>
@@ -1498,7 +1542,7 @@
       <c r="F31" s="87"/>
       <c r="G31" s="3"/>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A32" s="3"/>
       <c r="B32" s="8" t="s">
         <v>38</v>
@@ -1511,7 +1555,7 @@
       <c r="F32" s="87"/>
       <c r="G32" s="3"/>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A33" s="3"/>
       <c r="B33" s="10" t="s">
         <v>37</v>
@@ -1524,7 +1568,7 @@
       <c r="F33" s="87"/>
       <c r="G33" s="3"/>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A34" s="3"/>
       <c r="B34" s="8" t="s">
         <v>33</v>
@@ -1537,7 +1581,7 @@
       <c r="F34" s="87"/>
       <c r="G34" s="3"/>
     </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A35" s="3"/>
       <c r="B35" s="8" t="s">
         <v>39</v>
@@ -1550,7 +1594,7 @@
       <c r="F35" s="90"/>
       <c r="G35" s="3"/>
     </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A36" s="3"/>
       <c r="B36" s="8" t="s">
         <v>40</v>
@@ -1565,7 +1609,7 @@
       <c r="F36" s="7"/>
       <c r="G36" s="3"/>
     </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A37" s="3"/>
       <c r="B37" s="8" t="s">
         <v>30</v>
@@ -1580,7 +1624,7 @@
       <c r="F37" s="7"/>
       <c r="G37" s="3"/>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A38" s="3"/>
       <c r="B38" s="8"/>
       <c r="C38" s="3"/>
@@ -1589,7 +1633,7 @@
       <c r="F38" s="11"/>
       <c r="G38" s="3"/>
     </row>
-    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A39" s="3"/>
       <c r="B39" s="64" t="s">
         <v>13</v>
@@ -1600,7 +1644,7 @@
       <c r="F39" s="66"/>
       <c r="G39" s="3"/>
     </row>
-    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A40" s="3"/>
       <c r="B40" s="67"/>
       <c r="C40" s="68"/>
@@ -1609,7 +1653,7 @@
       <c r="F40" s="69"/>
       <c r="G40" s="3"/>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A41" s="3"/>
       <c r="B41" s="67"/>
       <c r="C41" s="68"/>
@@ -1618,7 +1662,7 @@
       <c r="F41" s="69"/>
       <c r="G41" s="3"/>
     </row>
-    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A42" s="3"/>
       <c r="B42" s="70"/>
       <c r="C42" s="71"/>
@@ -1627,7 +1671,7 @@
       <c r="F42" s="72"/>
       <c r="G42" s="3"/>
     </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A43" s="3"/>
       <c r="B43" s="8"/>
       <c r="C43" s="3"/>
@@ -1636,7 +1680,7 @@
       <c r="F43" s="9"/>
       <c r="G43" s="3"/>
     </row>
-    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A44" s="3"/>
       <c r="B44" s="58" t="s">
         <v>20</v>
@@ -1647,7 +1691,7 @@
       <c r="F44" s="60"/>
       <c r="G44" s="3"/>
     </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A45" s="3"/>
       <c r="B45" s="3"/>
       <c r="C45" s="3"/>
@@ -1656,7 +1700,7 @@
       <c r="F45" s="3"/>
       <c r="G45" s="3"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A46" s="3"/>
       <c r="B46" s="3"/>
       <c r="C46" s="3"/>
@@ -1878,20 +1922,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="06db5d4c-5cd4-4b65-ada8-b9ede3fff37f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="06db5d4c-5cd4-4b65-ada8-b9ede3fff37f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1913,14 +1957,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B60B9A07-1B61-4B18-979A-BFF9F350407D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A24E881E-BC61-42B4-887E-69DAA231223A}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
@@ -1934,4 +1970,12 @@
     <ds:schemaRef ds:uri="06db5d4c-5cd4-4b65-ada8-b9ede3fff37f"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B60B9A07-1B61-4B18-979A-BFF9F350407D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>